<commit_message>
Update lots of notes
</commit_message>
<xml_diff>
--- a/notebook/atlanticCodProject.xlsx
+++ b/notebook/atlanticCodProject.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saraschaal/Documents/Northeastern/LotterhosLab/Research/Bioinformatics/notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EF7984-8783-4648-A7D4-FF28C0523C19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6A361A-A343-0745-B6FC-41322959AFB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{312B3E53-055D-E14C-A1D8-24812159EF07}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -196,7 +196,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -206,6 +206,14 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -233,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -243,11 +251,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,7 +574,7 @@
   <dimension ref="A1:Y38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,177 +660,221 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:25" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="8">
         <v>44250</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:25" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="8">
         <v>44252</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="8">
         <v>44287</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="8">
         <v>44287</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="8">
         <v>44275</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="8">
         <v>44284</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="8">
         <v>44275</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+    <row r="19" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>